<commit_message>
RDM-6660 - Validation for PageDisplayOrder field in CaseEventToFields
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/development/ccd/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15FBF900-808A-5D45-97C4-805446FDE65E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975E8CD4-7FB5-034B-AE66-70DBDE54057D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$1:$M$32</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -15568,7 +15568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -17616,8 +17616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17910,7 +17910,9 @@
       <c r="F7" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="3" t="s">
         <v>56</v>
@@ -17946,7 +17948,9 @@
       <c r="F8" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="3" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
RDM-6719: Add Banner Feature to CCD UI
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15FBF900-808A-5D45-97C4-805446FDE65E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C35E11C-9F4F-4548-A5FC-F5A0E40318A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="357">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1125,6 +1125,27 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
+  </si>
+  <si>
+    <t>http://localhost:3451/test</t>
+  </si>
+  <si>
+    <t>Click here to see it.&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Test Description</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1157,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1429,6 +1450,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1697,7 +1725,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1708,8 +1736,9 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1978,14 +2007,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="43" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 2 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -2420,7 +2452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2429,7 +2463,10 @@
     <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="43.83203125" style="1" customWidth="1"/>
-    <col min="6" max="10" width="8.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.83203125" style="1" customWidth="1"/>
     <col min="11" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2487,10 +2524,18 @@
       <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>353</v>
+      </c>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2507,10 +2552,18 @@
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="200" t="s">
+        <v>356</v>
+      </c>
+      <c r="H4" s="200" t="s">
+        <v>355</v>
+      </c>
+      <c r="I4" s="201" t="s">
+        <v>354</v>
+      </c>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2634,6 +2687,9 @@
       <c r="J14" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{857D2DD5-4C3B-7644-91E8-6336E95E1984}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -15568,7 +15624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the def file with Banner RDM-6719 changes and revert the old one to resolve merge conflict.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
@@ -1,46 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F90A6-9359-1C41-A65F-BFA334F61047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15FBF900-808A-5D45-97C4-805446FDE65E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
-    <sheet name="Banner" sheetId="24" r:id="rId2"/>
-    <sheet name="CaseType" sheetId="2" r:id="rId3"/>
-    <sheet name="CaseField" sheetId="3" r:id="rId4"/>
-    <sheet name="FixedLists" sheetId="4" r:id="rId5"/>
-    <sheet name="ComplexTypes" sheetId="5" r:id="rId6"/>
-    <sheet name="State" sheetId="6" r:id="rId7"/>
-    <sheet name="CaseEvent" sheetId="7" r:id="rId8"/>
-    <sheet name="CaseEventToFields" sheetId="8" r:id="rId9"/>
-    <sheet name="SearchInputFields" sheetId="9" r:id="rId10"/>
-    <sheet name="SearchResultFields" sheetId="10" r:id="rId11"/>
-    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId12"/>
-    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId13"/>
-    <sheet name="CaseTypeTab" sheetId="13" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId15"/>
-    <sheet name="CaseRoles" sheetId="20" r:id="rId16"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId17"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="23" r:id="rId19"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId21"/>
-    <sheet name="SearchAlias" sheetId="22" r:id="rId22"/>
+    <sheet name="CaseType" sheetId="2" r:id="rId2"/>
+    <sheet name="CaseField" sheetId="3" r:id="rId3"/>
+    <sheet name="FixedLists" sheetId="4" r:id="rId4"/>
+    <sheet name="ComplexTypes" sheetId="5" r:id="rId5"/>
+    <sheet name="State" sheetId="6" r:id="rId6"/>
+    <sheet name="CaseEvent" sheetId="7" r:id="rId7"/>
+    <sheet name="CaseEventToFields" sheetId="8" r:id="rId8"/>
+    <sheet name="SearchInputFields" sheetId="9" r:id="rId9"/>
+    <sheet name="SearchResultFields" sheetId="10" r:id="rId10"/>
+    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId11"/>
+    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId12"/>
+    <sheet name="CaseTypeTab" sheetId="13" r:id="rId13"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId14"/>
+    <sheet name="CaseRoles" sheetId="20" r:id="rId15"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
+    <sheet name="AuthorisationComplexType" sheetId="23" r:id="rId18"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId20"/>
+    <sheet name="SearchAlias" sheetId="22" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId23"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CaseField!$A$1:$M$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$1:$M$32</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="350">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1126,39 +1125,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>Banner</t>
-  </si>
-  <si>
-    <t>BannerEnabled</t>
-  </si>
-  <si>
-    <t>BannerDescription</t>
-  </si>
-  <si>
-    <t>BannerUrlText</t>
-  </si>
-  <si>
-    <t>MaxLength:50</t>
-  </si>
-  <si>
-    <t>BannerUrl</t>
-  </si>
-  <si>
-    <t>URL. Mx Length: 1000</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Click here to see it.&gt;&gt;&gt;</t>
-  </si>
-  <si>
-    <t>http://localhost:3451/test</t>
-  </si>
-  <si>
-    <t>Test Description</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1136,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1463,19 +1429,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1744,7 +1697,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1755,9 +1708,8 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2026,17 +1978,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="43" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="10">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 2 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -2471,9 +2420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2696,342 +2643,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="47"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="F2" s="165" t="s">
-        <v>332</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>193</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="124" t="s">
-        <v>247</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="172"/>
-      <c r="G4" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="172"/>
-      <c r="G5" s="47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="172"/>
-      <c r="G6" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="172" t="s">
-        <v>249</v>
-      </c>
-      <c r="G7" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="172"/>
-      <c r="G8" s="47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="172"/>
-      <c r="G9" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="172"/>
-      <c r="G10" s="47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="172"/>
-      <c r="G11" s="47">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="172"/>
-      <c r="G12" s="47">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="172"/>
-      <c r="G13" s="47">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="172"/>
-      <c r="G14" s="47">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="53" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="172"/>
-      <c r="G15" s="47">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="172"/>
-      <c r="G16" s="47">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -3234,7 +2845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -3570,7 +3181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -3773,7 +3384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
@@ -4412,7 +4023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -4622,7 +4233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -4772,7 +4383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:IP12"/>
   <sheetViews>
@@ -7911,7 +7522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
@@ -8513,7 +8124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -8692,328 +8303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A1F88E-5CB0-9F47-9415-593D73C5FD9E}">
-  <dimension ref="A1:N17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="7"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A4" s="117" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="117" t="s">
-        <v>357</v>
-      </c>
-      <c r="C4" s="201" t="s">
-        <v>360</v>
-      </c>
-      <c r="D4" s="201" t="s">
-        <v>358</v>
-      </c>
-      <c r="E4" s="200" t="s">
-        <v>359</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A5" s="15"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A6" s="9"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A7" s="9"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A11" s="21"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A12" s="21"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A16" s="21"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{776E281B-4319-EE40-8BD3-3BD2915582CB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:IU15"/>
   <sheetViews>
@@ -13041,7 +12331,375 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="14" width="8.83203125" style="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" ht="74" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="9"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="21"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="21"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="21"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="21"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="21"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="21"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:IU15"/>
   <sheetViews>
@@ -13925,7 +13583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -14039,374 +13697,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="14" width="8.83203125" style="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" ht="74" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="9">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="9">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="9"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="9"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="21"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="21"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="21"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W42"/>
   <sheetViews>
@@ -15917,7 +15207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -16274,12 +15564,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17244,7 +16534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -17624,7 +16914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
@@ -18322,7 +17612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
@@ -19110,4 +18400,340 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
+    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="47"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="165" t="s">
+        <v>332</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="124" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="172"/>
+      <c r="G4" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="172"/>
+      <c r="G5" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="172"/>
+      <c r="G6" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="172" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="172"/>
+      <c r="G8" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="52"/>
+      <c r="C9" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="172"/>
+      <c r="G9" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="172"/>
+      <c r="G10" s="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="172"/>
+      <c r="G11" s="47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="172"/>
+      <c r="G12" s="47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="172"/>
+      <c r="G13" s="47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="172"/>
+      <c r="G14" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="172"/>
+      <c r="G15" s="47">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="52">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="52"/>
+      <c r="C16" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="172"/>
+      <c r="G16" s="47">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RDM-5690 - verified LAST_STATE_MODIFIED_DATE in the integration test
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V46_RDM-4324.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sateesh/moj/workspace/ccd/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F90A6-9359-1C41-A65F-BFA334F61047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5387591A-61CB-8942-B6E4-8BF0C2347A08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28020" windowHeight="16640" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="363">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1159,6 +1159,12 @@
   </si>
   <si>
     <t>Test Description</t>
+  </si>
+  <si>
+    <t>[LAST_STATE_MODIFIED_DATE]</t>
+  </si>
+  <si>
+    <t>Last State Modified Date</t>
   </si>
 </sst>
 </file>
@@ -3033,10 +3039,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3172,19 +3178,17 @@
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>71</v>
+        <v>361</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="172" t="s">
-        <v>249</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="F7" s="172"/>
       <c r="G7" s="47">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,14 +3200,16 @@
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>218</v>
-      </c>
-      <c r="F8" s="172"/>
+        <v>72</v>
+      </c>
+      <c r="F8" s="172" t="s">
+        <v>249</v>
+      </c>
       <c r="G8" s="47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3215,13 +3221,32 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
       <c r="F9" s="172"/>
       <c r="G9" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="54">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="172"/>
+      <c r="G10" s="47">
         <v>1</v>
       </c>
     </row>
@@ -8696,7 +8721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A1F88E-5CB0-9F47-9415-593D73C5FD9E}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8727,7 +8752,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>

</xml_diff>